<commit_message>
scrum file redundancy eliminated and with messv1 merged:-)
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_green.xlsx
+++ b/doc/task10/scrum_green.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="120" windowWidth="29040" windowHeight="15360"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="23720" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Effort Actual</t>
   </si>
   <si>
-    <t>UI, Controller</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -100,19 +97,7 @@
     <t>Der Patient kann seine definierten Skills -Funktion aufrufen</t>
   </si>
   <si>
-    <t>70h</t>
-  </si>
-  <si>
-    <t>150h</t>
-  </si>
-  <si>
-    <t>Persistent Storage</t>
-  </si>
-  <si>
-    <t>Store for the different Personal Data</t>
-  </si>
-  <si>
-    <t>80h</t>
+    <t>Package Diagram</t>
   </si>
   <si>
     <t>System Architecture</t>
@@ -203,86 +188,167 @@
     </r>
   </si>
   <si>
+    <t>Creating a UML package diagram to show the high-level structure of application.</t>
+  </si>
+  <si>
     <t>gnagj1</t>
   </si>
   <si>
-    <t>Package Diagram</t>
-  </si>
-  <si>
-    <t>Creating a UML package diagram to show the high-level structure of application.</t>
-  </si>
-  <si>
     <t>vonkc2</t>
   </si>
   <si>
+    <t xml:space="preserve">Mainview </t>
+  </si>
+  <si>
+    <t>Helpview</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Create a Model based on the Requirements for the Help Scenario</t>
+  </si>
+  <si>
     <t>Class Diagramm</t>
   </si>
   <si>
+    <t>LoginView</t>
+  </si>
+  <si>
+    <t>Create a Login view for later user specific Data Handling</t>
+  </si>
+  <si>
+    <t>User Data Manager</t>
+  </si>
+  <si>
+    <t>Create a Manager that gets the right Data based on the View and the logged in user</t>
+  </si>
+  <si>
+    <t>LoginManager</t>
+  </si>
+  <si>
+    <t>Based on the Login Data given the Manager must grant access or dissalow by checking data from database</t>
+  </si>
+  <si>
     <t>Create a Class Diagram / Domain Diagram for classes required</t>
   </si>
   <si>
-    <t xml:space="preserve">Mainview </t>
-  </si>
-  <si>
     <t>Create the Mainview of the Application in which the different views are displayed and a ViewManager</t>
   </si>
   <si>
-    <t>Helpview</t>
+    <t>70h</t>
+  </si>
+  <si>
+    <t>MedicView</t>
+  </si>
+  <si>
+    <t>Persistent Storage</t>
+  </si>
+  <si>
+    <t>Store for the different Personal Data</t>
+  </si>
+  <si>
+    <t>SkillsView</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Running Total Effort Org. </t>
+  </si>
+  <si>
+    <t>Running Total Effort Upd.</t>
+  </si>
+  <si>
+    <t>Running Total Effort Act.</t>
+  </si>
+  <si>
+    <t>Data Model</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Test the current Application on Errors</t>
+  </si>
+  <si>
+    <t>Design the Data Model for the Persistent Storage</t>
+  </si>
+  <si>
+    <t>Data Access</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>UI, Persenter</t>
+  </si>
+  <si>
+    <t>Create the Database Access Component, implementing the DataAccess Interface</t>
+  </si>
+  <si>
+    <t>DataAccess</t>
+  </si>
+  <si>
+    <t>Reminder</t>
+  </si>
+  <si>
+    <t>Create the MedicView with its Presenter and also beginn with the corresponding Settings view</t>
+  </si>
+  <si>
+    <t>Create the SkillsView with its Presenter and also beginn with the corresponding Settings view</t>
+  </si>
+  <si>
+    <t>ReminderComponent, Calendar</t>
+  </si>
+  <si>
+    <t>Reminder for due times to take medication, for each user and selected medic a timer needs to be created</t>
+  </si>
+  <si>
+    <t>Edit the Model to store the medication data</t>
+  </si>
+  <si>
+    <t>Solution to Push Reminder to User when not logged in.</t>
+  </si>
+  <si>
+    <t>work in prorgress</t>
+  </si>
+  <si>
+    <t>RemeinderComponent</t>
+  </si>
+  <si>
+    <t>60h</t>
+  </si>
+  <si>
+    <t>20h</t>
+  </si>
+  <si>
+    <t>40h</t>
+  </si>
+  <si>
+    <t>messv1</t>
+  </si>
+  <si>
+    <t>vandj2</t>
   </si>
   <si>
     <t>Create the Helpview with its Controller and also beginn with the corresponding Settings view</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Create a Model based on the Requirements for the Help Scenario</t>
+    <t>UI, Controller</t>
+  </si>
+  <si>
+    <t>medim1</t>
   </si>
   <si>
     <t>BLL</t>
   </si>
   <si>
-    <t>LoginView</t>
-  </si>
-  <si>
-    <t>Create a Login view for later user specific Data Handling</t>
-  </si>
-  <si>
-    <t>User Data Manager</t>
-  </si>
-  <si>
-    <t>Create a Manager that gets the right Data based on the View and the logged in user</t>
-  </si>
-  <si>
-    <t>LoginManager</t>
-  </si>
-  <si>
-    <t>Based on the Login Data given the Manager must grant access or dissalow by checking data from database</t>
-  </si>
-  <si>
-    <t>MedicView</t>
-  </si>
-  <si>
-    <t>Create the MedicView with its Controller and also beginn with the corresponding Settings view</t>
-  </si>
-  <si>
-    <t>SkillsView</t>
-  </si>
-  <si>
-    <t>Create the SkillsView with its Controller and also beginn with the corresponding Settings view</t>
-  </si>
-  <si>
-    <t>62h pro Person</t>
-  </si>
-  <si>
-    <t>12.5h pro Woche / Person :-(</t>
+    <t>dagde1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,8 +380,24 @@
       <name val="Orator Std Slanted"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +407,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,10 +426,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -358,8 +480,49 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="35">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -659,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -691,10 +854,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>14</v>
@@ -708,16 +871,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -725,16 +891,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -742,16 +911,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -759,26 +931,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="E9" t="s">
-        <v>57</v>
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -797,10 +962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -808,17 +973,20 @@
     <col min="1" max="1" width="6.1640625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="46" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,10 +1009,10 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -852,8 +1020,17 @@
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="78">
+      <c r="M1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="78">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -861,16 +1038,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -878,11 +1055,23 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="28">
+      <c r="M2">
+        <f>SUM(H$2:H2)</f>
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <f>SUM(I$2:I2)</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>SUM(J$2:J2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="28">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -890,16 +1079,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -907,11 +1096,23 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="M3">
+        <f>SUM(H$2:H3)</f>
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <f>SUM(I$2:I3)</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>SUM(J$2:J3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="28">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -919,13 +1120,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -933,11 +1137,23 @@
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="K4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="28">
+      <c r="K4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <f>SUM(H$2:H4)</f>
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <f>SUM(I$2:I4)</f>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>SUM(J$2:J4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="28">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -945,13 +1161,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -959,11 +1178,23 @@
       <c r="H5">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="28">
+      <c r="K5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <f>SUM(H$2:H5)</f>
+        <v>14</v>
+      </c>
+      <c r="N5">
+        <f>SUM(I$2:I5)</f>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>SUM(J$2:J5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="28">
       <c r="A6">
         <v>1.5</v>
       </c>
@@ -971,13 +1202,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -985,11 +1219,23 @@
       <c r="H6">
         <v>8</v>
       </c>
-      <c r="K6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="K6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <f>SUM(H$2:H6)</f>
+        <v>22</v>
+      </c>
+      <c r="N6">
+        <f>SUM(I$2:I6)</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>SUM(J$2:J6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="28">
       <c r="A7">
         <v>1.6</v>
       </c>
@@ -997,13 +1243,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -1011,11 +1260,23 @@
       <c r="H7">
         <v>4</v>
       </c>
-      <c r="K7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="K7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7">
+        <f>SUM(H$2:H7)</f>
+        <v>26</v>
+      </c>
+      <c r="N7">
+        <f>SUM(I$2:I7)</f>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>SUM(J$2:J7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>1.7</v>
       </c>
@@ -1023,13 +1284,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
@@ -1037,11 +1301,23 @@
       <c r="H8">
         <v>6</v>
       </c>
-      <c r="K8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="28">
+      <c r="K8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <f>SUM(H$2:H8)</f>
+        <v>32</v>
+      </c>
+      <c r="N8">
+        <f>SUM(I$2:I8)</f>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>SUM(J$2:J8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="28">
       <c r="A9">
         <v>1.8</v>
       </c>
@@ -1049,13 +1325,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -1063,11 +1342,23 @@
       <c r="H9">
         <v>19</v>
       </c>
-      <c r="K9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="28">
+      <c r="K9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <f>SUM(H$2:H9)</f>
+        <v>51</v>
+      </c>
+      <c r="N9">
+        <f>SUM(I$2:I9)</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>SUM(J$2:J9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="28">
       <c r="A10">
         <v>1.9</v>
       </c>
@@ -1075,13 +1366,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -1089,102 +1383,373 @@
       <c r="H10">
         <v>19</v>
       </c>
-      <c r="K10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="28">
-      <c r="A11">
+      <c r="K10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <f>SUM(H$2:H10)</f>
+        <v>70</v>
+      </c>
+      <c r="N10">
+        <f>SUM(I$2:I10)</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>SUM(J$2:J10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="8" customFormat="1">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" ht="28">
+      <c r="A12">
         <v>2.1</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="28">
-      <c r="A12">
-        <v>3.1</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <f>SUM(H$12:H12)</f>
+        <v>16</v>
+      </c>
+      <c r="N12">
+        <f>SUM(I$12:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>SUM(J$12:J12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="28">
       <c r="A13">
-        <v>2.2999999999999998</v>
+        <v>3.1</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="K13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <f>SUM(H$12:H13)</f>
+        <v>24</v>
+      </c>
+      <c r="N13">
+        <f>SUM(I$12:I13)</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>SUM(J$12:J13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="K14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <f>SUM(H$12:H14)</f>
+        <v>30</v>
+      </c>
+      <c r="N14">
+        <f>SUM(I$12:I14)</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>SUM(J$12:J14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="28">
       <c r="A15">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="K15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15">
+        <f>SUM(H$12:H15)</f>
+        <v>50</v>
+      </c>
+      <c r="N15">
+        <f>SUM(I$12:I15)</f>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>SUM(J$12:J15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" customFormat="1">
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <f>SUM(H$12:H16)</f>
+        <v>70</v>
+      </c>
+      <c r="N16">
+        <f>SUM(I$12:I16)</f>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>SUM(J$12:J16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" customFormat="1">
-      <c r="A18">
-        <v>2.8</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" customFormat="1">
-      <c r="A19">
-        <v>2.9</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="K17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <f>SUM(H$12:H17)</f>
+        <v>80</v>
+      </c>
+      <c r="N17">
+        <f>SUM(I$12:I17)</f>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>SUM(J$12:J17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="8" customFormat="1">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <f>SUM(H$22:H22)</f>
+        <v>12</v>
+      </c>
+      <c r="N22">
+        <f>SUM(I$12:I22)</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>SUM(J$12:J22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="28">
+      <c r="A23">
+        <v>4.2</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>18</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23">
+        <f>SUM(H$22:H23)</f>
+        <v>30</v>
+      </c>
+      <c r="N23">
+        <f>SUM(I$12:I23)</f>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>SUM(J$12:J23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24">
+        <v>4.3</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="K24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24">
+        <f>SUM(H$22:H24)</f>
+        <v>40</v>
+      </c>
+      <c r="N24">
+        <f>SUM(I$12:I24)</f>
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>SUM(J$12:J24)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated product and sprint log
</commit_message>
<xml_diff>
--- a/doc/task10/scrum_green.xlsx
+++ b/doc/task10/scrum_green.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="0" windowWidth="23720" windowHeight="19500"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="23720" windowHeight="19500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -49,9 +49,6 @@
     <t>waiting</t>
   </si>
   <si>
-    <t>work in progress</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -97,100 +94,6 @@
     <t>Der Patient kann seine definierten Skills -Funktion aufrufen</t>
   </si>
   <si>
-    <t>Package Diagram</t>
-  </si>
-  <si>
-    <t>System Architecture</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">design a software architecture taking into account
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Orator Std Slanted"/>
-        <family val="2"/>
-      </rPr>
-      <t>▶</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> system requirements
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Orator Std Slanted"/>
-        <family val="2"/>
-      </rPr>
-      <t>▶</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> incl. the need for persistent data storage
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Orator Std Slanted"/>
-        <family val="2"/>
-      </rPr>
-      <t>▶</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> architectural design patterns
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Orator Std Slanted"/>
-        <family val="2"/>
-      </rPr>
-      <t>▶</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the Vaadin framework</t>
-    </r>
-  </si>
-  <si>
-    <t>Creating a UML package diagram to show the high-level structure of application.</t>
-  </si>
-  <si>
     <t>gnagj1</t>
   </si>
   <si>
@@ -209,9 +112,6 @@
     <t>Create a Model based on the Requirements for the Help Scenario</t>
   </si>
   <si>
-    <t>Class Diagramm</t>
-  </si>
-  <si>
     <t>LoginView</t>
   </si>
   <si>
@@ -230,24 +130,12 @@
     <t>Based on the Login Data given the Manager must grant access or dissalow by checking data from database</t>
   </si>
   <si>
-    <t>Create a Class Diagram / Domain Diagram for classes required</t>
-  </si>
-  <si>
     <t>Create the Mainview of the Application in which the different views are displayed and a ViewManager</t>
   </si>
   <si>
-    <t>70h</t>
-  </si>
-  <si>
     <t>MedicView</t>
   </si>
   <si>
-    <t>Persistent Storage</t>
-  </si>
-  <si>
-    <t>Store for the different Personal Data</t>
-  </si>
-  <si>
     <t>SkillsView</t>
   </si>
   <si>
@@ -314,24 +202,12 @@
     <t>RemeinderComponent</t>
   </si>
   <si>
-    <t>60h</t>
-  </si>
-  <si>
-    <t>20h</t>
-  </si>
-  <si>
     <t>40h</t>
   </si>
   <si>
-    <t>messv1</t>
-  </si>
-  <si>
     <t>vandj2</t>
   </si>
   <si>
-    <t>Create the Helpview with its Controller and also beginn with the corresponding Settings view</t>
-  </si>
-  <si>
     <t>UI, Controller</t>
   </si>
   <si>
@@ -342,13 +218,37 @@
   </si>
   <si>
     <t>dagde1</t>
+  </si>
+  <si>
+    <t>80h</t>
+  </si>
+  <si>
+    <t>Help Settings View</t>
+  </si>
+  <si>
+    <t>Create the Helpview with its Controller and also beginn with the corresponding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings view </t>
+  </si>
+  <si>
+    <t>UI, Presenter</t>
+  </si>
+  <si>
+    <t>UI, Presneter</t>
+  </si>
+  <si>
+    <t>Mockup Data</t>
+  </si>
+  <si>
+    <t>Create Mockup data in the Model and the corresponding Entities (ContactPerson)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,12 +273,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="TimesNewRomanPSMT"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Orator Std Slanted"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -426,42 +320,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -488,7 +394,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="47">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -506,6 +412,12 @@
     <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -523,6 +435,12 @@
     <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -822,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -845,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -854,13 +772,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -871,19 +789,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -891,16 +809,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
@@ -911,38 +829,18 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -964,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K10"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -973,12 +871,12 @@
     <col min="1" max="1" width="6.1640625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="46" style="7" customWidth="1"/>
+    <col min="4" max="4" width="31.5" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" customWidth="1"/>
     <col min="12" max="12" width="5.6640625" customWidth="1"/>
@@ -991,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1000,37 +898,37 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="78">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="42">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1041,26 +939,26 @@
         <v>26</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M2">
         <f>SUM(H$2:H2)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N2">
         <f>SUM(I$2:I2)</f>
@@ -1079,40 +977,40 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M3">
-        <f>SUM(H$2:H3)</f>
-        <v>2</v>
+        <f>SUM(H$2:H5)</f>
+        <v>18</v>
       </c>
       <c r="N3">
-        <f>SUM(I$2:I3)</f>
+        <f>SUM(I$2:I5)</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f>SUM(J$2:J3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="28">
+        <f>SUM(J$2:J5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -1120,40 +1018,17 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4">
-        <f>SUM(H$2:H4)</f>
-        <v>4</v>
-      </c>
-      <c r="N4">
-        <f>SUM(I$2:I4)</f>
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <f>SUM(J$2:J4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="28">
+        <v>70</v>
+      </c>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:15" ht="42">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -1161,38 +1036,15 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5">
-        <f>SUM(H$2:H5)</f>
-        <v>14</v>
-      </c>
-      <c r="N5">
-        <f>SUM(I$2:I5)</f>
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <f>SUM(J$2:J5)</f>
-        <v>0</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:15" ht="28">
       <c r="A6">
@@ -1202,36 +1054,36 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>8</v>
       </c>
       <c r="M6">
-        <f>SUM(H$2:H6)</f>
-        <v>22</v>
+        <f>SUM(H$2:H7)</f>
+        <v>28</v>
       </c>
       <c r="N6">
-        <f>SUM(I$2:I6)</f>
+        <f>SUM(I$2:I7)</f>
         <v>0</v>
       </c>
       <c r="O6">
-        <f>SUM(J$2:J6)</f>
+        <f>SUM(J$2:J7)</f>
         <v>0</v>
       </c>
     </row>
@@ -1243,16 +1095,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -1265,7 +1117,7 @@
       </c>
       <c r="M7">
         <f>SUM(H$2:H7)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N7">
         <f>SUM(I$2:I7)</f>
@@ -1276,7 +1128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="42">
       <c r="A8">
         <v>1.7</v>
       </c>
@@ -1284,29 +1136,29 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="M8">
         <f>SUM(H$2:H8)</f>
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="N8">
         <f>SUM(I$2:I8)</f>
@@ -1317,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="28">
+    <row r="9" spans="1:15" ht="42">
       <c r="A9">
         <v>1.8</v>
       </c>
@@ -1325,16 +1177,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -1347,7 +1199,7 @@
       </c>
       <c r="M9">
         <f>SUM(H$2:H9)</f>
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="N9">
         <f>SUM(I$2:I9)</f>
@@ -1358,51 +1210,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="28">
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>1.9</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10">
-        <v>19</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10">
-        <f>SUM(H$2:H10)</f>
-        <v>70</v>
-      </c>
-      <c r="N10">
-        <f>SUM(I$2:I10)</f>
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <f>SUM(J$2:J10)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:15" s="8" customFormat="1">
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:15" ht="28">
+    <row r="12" spans="1:15" ht="42">
       <c r="A12">
         <v>2.1</v>
       </c>
@@ -1410,13 +1226,13 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -1440,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="28">
+    <row r="13" spans="1:15" ht="42">
       <c r="A13">
         <v>3.1</v>
       </c>
@@ -1448,13 +1264,13 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
         <v>48</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
@@ -1486,13 +1302,13 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
@@ -1516,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="28">
+    <row r="15" spans="1:15" ht="42">
       <c r="A15">
         <v>2.4</v>
       </c>
@@ -1524,13 +1340,13 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -1554,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" ht="28">
       <c r="A16">
         <v>2.5</v>
       </c>
@@ -1562,13 +1378,13 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G16" t="s">
         <v>6</v>
@@ -1592,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" ht="28">
       <c r="A17">
         <v>2.6</v>
       </c>
@@ -1600,13 +1416,13 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G17" t="s">
         <v>6</v>
@@ -1633,7 +1449,7 @@
     <row r="21" spans="1:15" s="8" customFormat="1">
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" ht="28">
       <c r="A22">
         <v>4.0999999999999996</v>
       </c>
@@ -1641,13 +1457,13 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
@@ -1671,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="28">
+    <row r="23" spans="1:15" ht="42">
       <c r="A23">
         <v>4.2</v>
       </c>
@@ -1679,13 +1495,13 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
@@ -1717,13 +1533,13 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>

</xml_diff>